<commit_message>
10.11.23 Filter Test completed.
</commit_message>
<xml_diff>
--- a/src/test/manual/Swag Labs-Test Scenarios.xlsx
+++ b/src/test/manual/Swag Labs-Test Scenarios.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="3765" tabRatio="670" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="3765" tabRatio="670" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="872" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="439">
   <si>
     <t>Project Name</t>
   </si>
@@ -5593,7 +5593,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="31" x14ac:knownFonts="1">
+  <fonts count="32" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5821,8 +5821,16 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="72"/>
+      <color theme="9" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5851,6 +5859,12 @@
         <fgColor rgb="FFFFC7CE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -5971,7 +5985,7 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="65">
+  <cellXfs count="66">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -6158,6 +6172,9 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -6450,7 +6467,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -6595,7 +6612,7 @@
         <v>3</v>
       </c>
       <c r="D13" s="7">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="E13" s="2"/>
     </row>
@@ -9242,8 +9259,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="X13" sqref="X13"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
@@ -10011,8 +10028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
@@ -10092,7 +10109,7 @@
       <c r="I2" s="47">
         <v>0</v>
       </c>
-      <c r="J2" s="58" t="s">
+      <c r="J2" s="65" t="s">
         <v>437</v>
       </c>
       <c r="K2" s="32"/>
@@ -10123,7 +10140,7 @@
       <c r="I3" s="47">
         <v>1</v>
       </c>
-      <c r="J3" s="58" t="s">
+      <c r="J3" s="65" t="s">
         <v>437</v>
       </c>
       <c r="K3" s="32"/>
@@ -10154,7 +10171,7 @@
       <c r="I4" s="50">
         <v>0</v>
       </c>
-      <c r="J4" s="58" t="s">
+      <c r="J4" s="65" t="s">
         <v>437</v>
       </c>
       <c r="K4" s="32"/>
@@ -10185,7 +10202,7 @@
       <c r="I5" s="50">
         <v>2</v>
       </c>
-      <c r="J5" s="58" t="s">
+      <c r="J5" s="65" t="s">
         <v>437</v>
       </c>
       <c r="K5" s="32"/>
@@ -10528,8 +10545,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+    <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
@@ -10609,7 +10626,9 @@
       <c r="I2" s="47">
         <v>1</v>
       </c>
-      <c r="J2" s="32"/>
+      <c r="J2" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="K2" s="32"/>
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
@@ -10638,7 +10657,9 @@
       <c r="I3" s="47">
         <v>1</v>
       </c>
-      <c r="J3" s="32"/>
+      <c r="J3" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="K3" s="32"/>
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -10667,7 +10688,9 @@
       <c r="I4" s="47">
         <v>1</v>
       </c>
-      <c r="J4" s="32"/>
+      <c r="J4" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="K4" s="32"/>
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -10696,7 +10719,9 @@
       <c r="I5" s="47">
         <v>1</v>
       </c>
-      <c r="J5" s="32"/>
+      <c r="J5" s="65" t="s">
+        <v>437</v>
+      </c>
       <c r="K5" s="32"/>
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
All Items Test 12.11.2023
</commit_message>
<xml_diff>
--- a/src/test/manual/Swag Labs-Test Scenarios.xlsx
+++ b/src/test/manual/Swag Labs-Test Scenarios.xlsx
@@ -1,15 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Desktop\shelf1\Swag Labs\automation\Swag Labs\SwagLabs\src\test\manual\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="6" rupBuild="4505"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="3765" tabRatio="670" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10215" windowHeight="3765" tabRatio="670" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Test Scenarios" sheetId="1" r:id="rId1"/>
@@ -27,8 +22,9 @@
     <sheet name="Heder,Footer" sheetId="13" r:id="rId13"/>
   </sheets>
   <calcPr calcId="124519"/>
-  <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+  <fileRecoveryPr repairLoad="1"/>
+  <extLst xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
   </extLst>
@@ -36,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="876" uniqueCount="439">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="877" uniqueCount="441">
   <si>
     <t>Project Name</t>
   </si>
@@ -5587,13 +5583,19 @@
   </si>
   <si>
     <t>Validate the Logout functionality in all the supported environments</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>1. Home (All Products) page should be opened.                     2. Menu bar should be closed.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="32" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="33">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -5829,8 +5831,16 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="72"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="7">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -5865,6 +5875,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFF9393"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="9">
     <border>
@@ -5985,7 +6001,7 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="25" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="66">
+  <cellXfs count="67">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
@@ -6164,6 +6180,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
@@ -6173,7 +6192,7 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="3" xfId="2" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -6187,6 +6206,8 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF9393"/>
+      <color rgb="FFEEA4BB"/>
       <color rgb="FFD1D1D1"/>
     </mruColors>
   </colors>
@@ -6244,7 +6265,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -6279,7 +6300,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -6456,21 +6477,21 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:E43"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+    <sheetView topLeftCell="B10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75"/>
   <cols>
     <col min="1" max="1" width="20.85546875" style="1" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="77" style="1" customWidth="1"/>
@@ -6480,25 +6501,25 @@
     <col min="6" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5">
       <c r="A1" s="2"/>
       <c r="B1" s="3"/>
       <c r="C1" s="2"/>
       <c r="D1" s="2"/>
       <c r="E1" s="2"/>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5">
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="62" t="s">
+      <c r="B2" s="63" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="63"/>
+      <c r="C2" s="64"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5">
       <c r="A3" s="25" t="s">
         <v>1</v>
       </c>
@@ -6509,7 +6530,7 @@
       <c r="D3" s="2"/>
       <c r="E3" s="2"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5">
       <c r="A4" s="25" t="s">
         <v>2</v>
       </c>
@@ -6520,43 +6541,43 @@
       <c r="D4" s="2"/>
       <c r="E4" s="2"/>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5">
       <c r="A5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="64" t="s">
+      <c r="B5" s="65" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="63"/>
+      <c r="C5" s="64"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5">
       <c r="D6" s="2"/>
       <c r="E6" s="2"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5">
       <c r="A7" s="2"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
       <c r="E7" s="2"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5">
       <c r="A8" s="2"/>
       <c r="B8" s="2"/>
       <c r="C8" s="2"/>
       <c r="D8" s="2"/>
       <c r="E8" s="2"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5">
       <c r="A9" s="2"/>
       <c r="B9" s="2"/>
       <c r="C9" s="2"/>
       <c r="D9" s="2"/>
       <c r="E9" s="2"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5">
       <c r="A10" s="26" t="s">
         <v>3</v>
       </c>
@@ -6571,7 +6592,7 @@
       </c>
       <c r="E10" s="2"/>
     </row>
-    <row r="11" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" ht="15.75">
       <c r="A11" s="5" t="s">
         <v>8</v>
       </c>
@@ -6586,7 +6607,7 @@
       </c>
       <c r="E11" s="2"/>
     </row>
-    <row r="12" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" ht="15.75">
       <c r="A12" s="5" t="s">
         <v>9</v>
       </c>
@@ -6601,7 +6622,7 @@
       </c>
       <c r="E12" s="2"/>
     </row>
-    <row r="13" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="15.75">
       <c r="A13" s="5" t="s">
         <v>10</v>
       </c>
@@ -6616,7 +6637,7 @@
       </c>
       <c r="E13" s="2"/>
     </row>
-    <row r="14" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="15.75">
       <c r="A14" s="5" t="s">
         <v>11</v>
       </c>
@@ -6631,7 +6652,7 @@
       </c>
       <c r="E14" s="2"/>
     </row>
-    <row r="15" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="16.5" customHeight="1">
       <c r="A15" s="5" t="s">
         <v>12</v>
       </c>
@@ -6646,7 +6667,7 @@
       </c>
       <c r="E15" s="2"/>
     </row>
-    <row r="16" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" ht="15.75">
       <c r="A16" s="5" t="s">
         <v>13</v>
       </c>
@@ -6661,7 +6682,7 @@
       </c>
       <c r="E16" s="2"/>
     </row>
-    <row r="17" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" ht="15.75">
       <c r="A17" s="5" t="s">
         <v>14</v>
       </c>
@@ -6676,7 +6697,7 @@
       </c>
       <c r="E17" s="2"/>
     </row>
-    <row r="18" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" ht="15.75">
       <c r="A18" s="5" t="s">
         <v>15</v>
       </c>
@@ -6691,7 +6712,7 @@
       </c>
       <c r="E18" s="2"/>
     </row>
-    <row r="19" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" ht="15.75">
       <c r="A19" s="5" t="s">
         <v>16</v>
       </c>
@@ -6706,7 +6727,7 @@
       </c>
       <c r="E19" s="2"/>
     </row>
-    <row r="20" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" ht="15.75">
       <c r="A20" s="5" t="s">
         <v>17</v>
       </c>
@@ -6721,7 +6742,7 @@
       </c>
       <c r="E20" s="2"/>
     </row>
-    <row r="21" spans="1:5" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" ht="16.5" customHeight="1">
       <c r="A21" s="11" t="s">
         <v>18</v>
       </c>
@@ -6736,7 +6757,7 @@
       </c>
       <c r="E21" s="2"/>
     </row>
-    <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" ht="15.75">
       <c r="A22" s="12" t="s">
         <v>367</v>
       </c>
@@ -6751,147 +6772,147 @@
       </c>
       <c r="E22" s="2"/>
     </row>
-    <row r="23" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" ht="15.75">
       <c r="A23" s="18"/>
       <c r="B23" s="19"/>
       <c r="C23" s="20"/>
       <c r="D23" s="21"/>
       <c r="E23" s="2"/>
     </row>
-    <row r="24" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" ht="15.75">
       <c r="A24" s="18"/>
       <c r="B24" s="19"/>
       <c r="C24" s="20"/>
       <c r="D24" s="21"/>
       <c r="E24" s="2"/>
     </row>
-    <row r="25" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" ht="15.75">
       <c r="A25" s="18"/>
       <c r="B25" s="19"/>
       <c r="C25" s="20"/>
       <c r="D25" s="21"/>
       <c r="E25" s="2"/>
     </row>
-    <row r="26" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" ht="15.75">
       <c r="A26" s="18"/>
       <c r="B26" s="19"/>
       <c r="C26" s="20"/>
       <c r="D26" s="21"/>
       <c r="E26" s="2"/>
     </row>
-    <row r="27" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" ht="15.75">
       <c r="A27" s="18"/>
       <c r="B27" s="19"/>
       <c r="C27" s="20"/>
       <c r="D27" s="21"/>
       <c r="E27" s="2"/>
     </row>
-    <row r="28" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" ht="15.75">
       <c r="A28" s="18"/>
       <c r="B28" s="19"/>
       <c r="C28" s="20"/>
       <c r="D28" s="21"/>
       <c r="E28" s="2"/>
     </row>
-    <row r="29" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" ht="15.75">
       <c r="A29" s="18"/>
       <c r="B29" s="19"/>
       <c r="C29" s="20"/>
       <c r="D29" s="21"/>
       <c r="E29" s="2"/>
     </row>
-    <row r="30" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" ht="15.75">
       <c r="A30" s="18"/>
       <c r="B30" s="19"/>
       <c r="C30" s="20"/>
       <c r="D30" s="21"/>
       <c r="E30" s="2"/>
     </row>
-    <row r="31" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" ht="15.75">
       <c r="A31" s="18"/>
       <c r="B31" s="19"/>
       <c r="C31" s="20"/>
       <c r="D31" s="21"/>
       <c r="E31" s="2"/>
     </row>
-    <row r="32" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" ht="15.75">
       <c r="A32" s="18"/>
       <c r="B32" s="19"/>
       <c r="C32" s="20"/>
       <c r="D32" s="21"/>
       <c r="E32" s="2"/>
     </row>
-    <row r="33" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" ht="15.75">
       <c r="A33" s="18"/>
       <c r="B33" s="19"/>
       <c r="C33" s="20"/>
       <c r="D33" s="21"/>
       <c r="E33" s="2"/>
     </row>
-    <row r="34" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" ht="15.75">
       <c r="A34" s="18"/>
       <c r="B34" s="19"/>
       <c r="C34" s="20"/>
       <c r="D34" s="21"/>
       <c r="E34" s="2"/>
     </row>
-    <row r="35" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" ht="15.75">
       <c r="A35" s="18"/>
       <c r="B35" s="19"/>
       <c r="C35" s="20"/>
       <c r="D35" s="21"/>
       <c r="E35" s="2"/>
     </row>
-    <row r="36" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="15.75">
       <c r="A36" s="18"/>
       <c r="B36" s="19"/>
       <c r="C36" s="20"/>
       <c r="D36" s="21"/>
       <c r="E36" s="2"/>
     </row>
-    <row r="37" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="15.75">
       <c r="A37" s="18"/>
       <c r="B37" s="19"/>
       <c r="C37" s="20"/>
       <c r="D37" s="21"/>
       <c r="E37" s="2"/>
     </row>
-    <row r="38" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="15.75">
       <c r="A38" s="18"/>
       <c r="B38" s="19"/>
       <c r="C38" s="20"/>
       <c r="D38" s="21"/>
       <c r="E38" s="2"/>
     </row>
-    <row r="39" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="15.75">
       <c r="A39" s="18"/>
       <c r="B39" s="19"/>
       <c r="C39" s="20"/>
       <c r="D39" s="21"/>
       <c r="E39" s="2"/>
     </row>
-    <row r="40" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="15.75">
       <c r="A40" s="18"/>
       <c r="B40" s="19"/>
       <c r="C40" s="20"/>
       <c r="D40" s="21"/>
       <c r="E40" s="2"/>
     </row>
-    <row r="41" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="15.75">
       <c r="A41" s="18"/>
       <c r="B41" s="19"/>
       <c r="C41" s="20"/>
       <c r="D41" s="21"/>
       <c r="E41" s="2"/>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5">
       <c r="A42" s="2"/>
       <c r="B42" s="2"/>
       <c r="C42" s="2"/>
       <c r="D42" s="2"/>
       <c r="E42" s="2"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5">
       <c r="A43" s="2"/>
       <c r="B43" s="2"/>
       <c r="C43" s="2"/>
@@ -6910,14 +6931,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -6933,7 +6954,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -6968,7 +6989,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>271</v>
       </c>
@@ -6997,7 +7018,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>272</v>
       </c>
@@ -7026,7 +7047,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>273</v>
       </c>
@@ -7055,7 +7076,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="157.5" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>274</v>
       </c>
@@ -7084,7 +7105,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>275</v>
       </c>
@@ -7113,7 +7134,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="117" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>276</v>
       </c>
@@ -7142,7 +7163,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="107.25" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>277</v>
       </c>
@@ -7171,7 +7192,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="127.5" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>278</v>
       </c>
@@ -7200,7 +7221,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="124.5" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>279</v>
       </c>
@@ -7229,7 +7250,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>280</v>
       </c>
@@ -7258,7 +7279,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>296</v>
       </c>
@@ -7287,7 +7308,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="213.75" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>301</v>
       </c>
@@ -7316,7 +7337,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1">
       <c r="A14" s="32" t="s">
         <v>309</v>
       </c>
@@ -7345,7 +7366,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="160.5" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>310</v>
       </c>
@@ -7374,7 +7395,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1">
       <c r="A16" s="32" t="s">
         <v>322</v>
       </c>
@@ -7403,7 +7424,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="153.75" customHeight="1">
       <c r="A17" s="32" t="s">
         <v>323</v>
       </c>
@@ -7432,7 +7453,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="155.25" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>324</v>
       </c>
@@ -7461,7 +7482,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="32"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -7474,7 +7495,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -7487,7 +7508,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -7500,7 +7521,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -7513,7 +7534,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -7526,7 +7547,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -7539,7 +7560,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -7552,7 +7573,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -7565,7 +7586,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -7578,7 +7599,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -7591,7 +7612,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -7611,14 +7632,14 @@
 </file>
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -7634,7 +7655,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -7669,7 +7690,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="135" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>328</v>
       </c>
@@ -7698,7 +7719,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="135" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>329</v>
       </c>
@@ -7727,7 +7748,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>330</v>
       </c>
@@ -7756,7 +7777,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="157.5" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>331</v>
       </c>
@@ -7785,7 +7806,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="132.75" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>332</v>
       </c>
@@ -7814,7 +7835,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="150" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>333</v>
       </c>
@@ -7843,7 +7864,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="162.75" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>334</v>
       </c>
@@ -7872,7 +7893,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="153" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>335</v>
       </c>
@@ -7901,7 +7922,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="156.75" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>336</v>
       </c>
@@ -7930,7 +7951,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="159.75" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>337</v>
       </c>
@@ -7959,7 +7980,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="42"/>
@@ -7972,7 +7993,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="213.75" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="44"/>
@@ -7985,7 +8006,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="44"/>
@@ -7998,7 +8019,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="160.5" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="44"/>
@@ -8011,7 +8032,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="44"/>
@@ -8024,7 +8045,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="153.75" customHeight="1">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="44"/>
@@ -8037,7 +8058,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="155.25" customHeight="1">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="44"/>
@@ -8050,7 +8071,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="32"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -8063,7 +8084,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -8076,7 +8097,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -8089,7 +8110,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -8102,7 +8123,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -8115,7 +8136,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -8128,7 +8149,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -8141,7 +8162,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -8154,7 +8175,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -8167,7 +8188,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -8180,7 +8201,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -8200,14 +8221,14 @@
 </file>
 
 <file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -8223,7 +8244,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -8258,7 +8279,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="153" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>373</v>
       </c>
@@ -8287,7 +8308,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="177" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>379</v>
       </c>
@@ -8314,7 +8335,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1">
       <c r="A4" s="32"/>
       <c r="B4" s="32"/>
       <c r="C4" s="44"/>
@@ -8327,7 +8348,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="157.5" customHeight="1">
       <c r="A5" s="32"/>
       <c r="B5" s="32"/>
       <c r="C5" s="44"/>
@@ -8340,7 +8361,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1">
       <c r="A6" s="32"/>
       <c r="B6" s="32"/>
       <c r="C6" s="44"/>
@@ -8353,7 +8374,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="117" customHeight="1">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="44"/>
@@ -8366,7 +8387,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="107.25" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="32"/>
       <c r="C8" s="44"/>
@@ -8379,7 +8400,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="127.5" customHeight="1">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
       <c r="C9" s="44"/>
@@ -8392,7 +8413,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="124.5" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="44"/>
@@ -8405,7 +8426,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="44"/>
@@ -8418,7 +8439,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="42"/>
@@ -8431,7 +8452,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="213.75" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="44"/>
@@ -8444,7 +8465,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="44"/>
@@ -8457,7 +8478,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="160.5" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="44"/>
@@ -8470,7 +8491,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="44"/>
@@ -8483,7 +8504,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="153.75" customHeight="1">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="44"/>
@@ -8496,7 +8517,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="155.25" customHeight="1">
       <c r="A18" s="32"/>
       <c r="B18" s="32"/>
       <c r="C18" s="44"/>
@@ -8509,7 +8530,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="32"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -8522,7 +8543,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -8535,7 +8556,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -8548,7 +8569,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -8561,7 +8582,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -8574,7 +8595,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -8587,7 +8608,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -8600,7 +8621,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -8613,7 +8634,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -8626,7 +8647,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -8639,7 +8660,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -8658,14 +8679,14 @@
 </file>
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -8681,7 +8702,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -8716,7 +8737,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>224</v>
       </c>
@@ -8745,7 +8766,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>225</v>
       </c>
@@ -8774,7 +8795,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>226</v>
       </c>
@@ -8803,7 +8824,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>227</v>
       </c>
@@ -8832,7 +8853,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>228</v>
       </c>
@@ -8859,7 +8880,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>229</v>
       </c>
@@ -8888,7 +8909,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>246</v>
       </c>
@@ -8915,7 +8936,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="105.75" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>247</v>
       </c>
@@ -8942,7 +8963,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>248</v>
       </c>
@@ -8969,7 +8990,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>401</v>
       </c>
@@ -8996,7 +9017,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>402</v>
       </c>
@@ -9023,7 +9044,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -9036,7 +9057,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -9049,7 +9070,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="150.75" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -9062,7 +9083,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -9075,7 +9096,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A17" s="42"/>
       <c r="B17" s="42"/>
       <c r="C17" s="32"/>
@@ -9088,7 +9109,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="32"/>
@@ -9101,7 +9122,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -9114,7 +9135,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -9127,7 +9148,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -9140,7 +9161,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -9153,7 +9174,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -9166,7 +9187,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -9179,7 +9200,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -9192,7 +9213,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -9205,7 +9226,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -9218,7 +9239,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -9231,7 +9252,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -9256,14 +9277,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+    <sheetView topLeftCell="B19" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -9279,7 +9300,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -9314,7 +9335,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A2" s="42" t="s">
         <v>40</v>
       </c>
@@ -9345,7 +9366,7 @@
       </c>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A3" s="42" t="s">
         <v>46</v>
       </c>
@@ -9376,7 +9397,7 @@
       </c>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A4" s="42" t="s">
         <v>48</v>
       </c>
@@ -9407,7 +9428,7 @@
       </c>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A5" s="42" t="s">
         <v>50</v>
       </c>
@@ -9438,7 +9459,7 @@
       </c>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>55</v>
       </c>
@@ -9469,7 +9490,7 @@
       </c>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>59</v>
       </c>
@@ -9500,7 +9521,7 @@
       </c>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>61</v>
       </c>
@@ -9531,7 +9552,7 @@
       </c>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="105.75" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>64</v>
       </c>
@@ -9562,7 +9583,7 @@
       </c>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="101.25" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>72</v>
       </c>
@@ -9593,7 +9614,7 @@
       </c>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32" t="s">
         <v>73</v>
       </c>
@@ -9624,7 +9645,7 @@
       </c>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="112.5" customHeight="1">
       <c r="A12" s="32" t="s">
         <v>76</v>
       </c>
@@ -9655,7 +9676,7 @@
       </c>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="175.5" customHeight="1">
       <c r="A13" s="32" t="s">
         <v>80</v>
       </c>
@@ -9686,7 +9707,7 @@
       </c>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A14" s="32" t="s">
         <v>83</v>
       </c>
@@ -9717,7 +9738,7 @@
       </c>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="150.75" customHeight="1">
       <c r="A15" s="32" t="s">
         <v>89</v>
       </c>
@@ -9748,7 +9769,7 @@
       </c>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1">
       <c r="A16" s="32" t="s">
         <v>90</v>
       </c>
@@ -9779,7 +9800,7 @@
       </c>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A17" s="32" t="s">
         <v>420</v>
       </c>
@@ -9810,7 +9831,7 @@
       </c>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="32" t="s">
         <v>421</v>
       </c>
@@ -9841,7 +9862,7 @@
       </c>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="168" customHeight="1">
       <c r="A19" s="32" t="s">
         <v>431</v>
       </c>
@@ -9872,7 +9893,7 @@
       </c>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="32" t="s">
         <v>432</v>
       </c>
@@ -9901,7 +9922,7 @@
       <c r="J20" s="58"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -9914,7 +9935,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -9927,7 +9948,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -9940,7 +9961,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -9953,7 +9974,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -9966,7 +9987,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -9979,7 +10000,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -9992,7 +10013,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -10005,7 +10026,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -10025,14 +10046,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -10048,7 +10069,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -10083,7 +10104,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="120" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="120" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>100</v>
       </c>
@@ -10109,12 +10130,12 @@
       <c r="I2" s="47">
         <v>0</v>
       </c>
-      <c r="J2" s="65" t="s">
+      <c r="J2" s="62" t="s">
         <v>437</v>
       </c>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="138" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>101</v>
       </c>
@@ -10140,12 +10161,12 @@
       <c r="I3" s="47">
         <v>1</v>
       </c>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="62" t="s">
         <v>437</v>
       </c>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="136.5" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>102</v>
       </c>
@@ -10171,12 +10192,12 @@
       <c r="I4" s="50">
         <v>0</v>
       </c>
-      <c r="J4" s="65" t="s">
+      <c r="J4" s="62" t="s">
         <v>437</v>
       </c>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="156" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>103</v>
       </c>
@@ -10202,12 +10223,12 @@
       <c r="I5" s="50">
         <v>2</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="62" t="s">
         <v>437</v>
       </c>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>104</v>
       </c>
@@ -10236,7 +10257,7 @@
       <c r="J6" s="58"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
@@ -10249,7 +10270,7 @@
       <c r="J7" s="58"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
@@ -10262,7 +10283,7 @@
       <c r="J8" s="58"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -10275,7 +10296,7 @@
       <c r="J9" s="58"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="42"/>
@@ -10288,7 +10309,7 @@
       <c r="J10" s="58"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="42"/>
@@ -10301,7 +10322,7 @@
       <c r="J11" s="58"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="42"/>
@@ -10314,7 +10335,7 @@
       <c r="J12" s="58"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -10327,7 +10348,7 @@
       <c r="J13" s="58"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -10340,7 +10361,7 @@
       <c r="J14" s="58"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -10353,7 +10374,7 @@
       <c r="J15" s="58"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -10366,7 +10387,7 @@
       <c r="J16" s="59"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -10379,7 +10400,7 @@
       <c r="J17" s="58"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="32"/>
@@ -10392,7 +10413,7 @@
       <c r="J18" s="58"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -10405,7 +10426,7 @@
       <c r="J19" s="58"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -10418,7 +10439,7 @@
       <c r="J20" s="58"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -10431,7 +10452,7 @@
       <c r="J21" s="60"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -10444,7 +10465,7 @@
       <c r="J22" s="60"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -10457,7 +10478,7 @@
       <c r="J23" s="60"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -10470,7 +10491,7 @@
       <c r="J24" s="60"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -10483,7 +10504,7 @@
       <c r="J25" s="60"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -10496,7 +10517,7 @@
       <c r="J26" s="60"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -10509,7 +10530,7 @@
       <c r="J27" s="60"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -10522,7 +10543,7 @@
       <c r="J28" s="60"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -10542,14 +10563,14 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -10565,7 +10586,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -10600,7 +10621,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="96.75" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>119</v>
       </c>
@@ -10626,12 +10647,12 @@
       <c r="I2" s="47">
         <v>1</v>
       </c>
-      <c r="J2" s="65" t="s">
+      <c r="J2" s="62" t="s">
         <v>437</v>
       </c>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>120</v>
       </c>
@@ -10657,12 +10678,12 @@
       <c r="I3" s="47">
         <v>1</v>
       </c>
-      <c r="J3" s="65" t="s">
+      <c r="J3" s="62" t="s">
         <v>437</v>
       </c>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>121</v>
       </c>
@@ -10688,12 +10709,12 @@
       <c r="I4" s="47">
         <v>1</v>
       </c>
-      <c r="J4" s="65" t="s">
+      <c r="J4" s="62" t="s">
         <v>437</v>
       </c>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="111.75" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>122</v>
       </c>
@@ -10719,12 +10740,12 @@
       <c r="I5" s="47">
         <v>1</v>
       </c>
-      <c r="J5" s="65" t="s">
+      <c r="J5" s="62" t="s">
         <v>437</v>
       </c>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A6" s="32"/>
       <c r="B6" s="32"/>
       <c r="C6" s="44"/>
@@ -10737,7 +10758,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
@@ -10750,7 +10771,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
@@ -10763,7 +10784,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -10776,7 +10797,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="42"/>
@@ -10789,7 +10810,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="42"/>
@@ -10802,7 +10823,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="42"/>
@@ -10815,7 +10836,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -10828,7 +10849,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -10841,7 +10862,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -10854,7 +10875,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -10867,7 +10888,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -10880,7 +10901,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="32"/>
@@ -10893,7 +10914,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -10906,7 +10927,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -10919,7 +10940,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -10932,7 +10953,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -10945,7 +10966,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -10958,7 +10979,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -10971,7 +10992,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -10984,7 +11005,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -10997,7 +11018,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -11010,7 +11031,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -11023,7 +11044,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -11042,14 +11063,14 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="E5" sqref="E5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -11065,7 +11086,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -11100,7 +11121,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="96.75" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>135</v>
       </c>
@@ -11120,16 +11141,18 @@
         <v>58</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>141</v>
+        <v>440</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="47">
         <v>0</v>
       </c>
-      <c r="J2" s="32"/>
+      <c r="J2" s="66" t="s">
+        <v>439</v>
+      </c>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>136</v>
       </c>
@@ -11158,7 +11181,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>137</v>
       </c>
@@ -11187,7 +11210,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="115.5" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>139</v>
       </c>
@@ -11216,7 +11239,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="139.5" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>138</v>
       </c>
@@ -11245,7 +11268,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="32"/>
@@ -11258,7 +11281,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
@@ -11271,7 +11294,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -11284,7 +11307,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="42"/>
@@ -11297,7 +11320,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="42"/>
@@ -11310,7 +11333,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="42"/>
@@ -11323,7 +11346,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -11336,7 +11359,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -11349,7 +11372,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -11362,7 +11385,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -11375,7 +11398,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -11388,7 +11411,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="32"/>
@@ -11401,7 +11424,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -11414,7 +11437,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -11427,7 +11450,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -11440,7 +11463,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -11453,7 +11476,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -11466,7 +11489,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -11479,7 +11502,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -11492,7 +11515,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -11505,7 +11528,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -11518,7 +11541,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -11531,7 +11554,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -11551,14 +11574,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -11574,7 +11597,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -11609,7 +11632,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="96.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="96.75" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>155</v>
       </c>
@@ -11638,7 +11661,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>156</v>
       </c>
@@ -11667,7 +11690,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>157</v>
       </c>
@@ -11696,7 +11719,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="115.5" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>158</v>
       </c>
@@ -11725,7 +11748,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>159</v>
       </c>
@@ -11754,7 +11777,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="44"/>
@@ -11767,7 +11790,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
@@ -11780,7 +11803,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -11793,7 +11816,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="42"/>
@@ -11806,7 +11829,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="42"/>
@@ -11819,7 +11842,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="42"/>
@@ -11832,7 +11855,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -11845,7 +11868,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -11858,7 +11881,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -11871,7 +11894,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -11884,7 +11907,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -11897,7 +11920,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="32"/>
@@ -11910,7 +11933,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -11923,7 +11946,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -11936,7 +11959,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -11949,7 +11972,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -11962,7 +11985,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -11975,7 +11998,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -11988,7 +12011,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -12001,7 +12024,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -12014,7 +12037,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -12027,7 +12050,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -12040,7 +12063,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -12060,14 +12083,14 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -12083,7 +12106,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -12118,7 +12141,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>176</v>
       </c>
@@ -12147,7 +12170,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>177</v>
       </c>
@@ -12176,7 +12199,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>178</v>
       </c>
@@ -12205,7 +12228,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="142.5" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>179</v>
       </c>
@@ -12234,7 +12257,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>180</v>
       </c>
@@ -12263,7 +12286,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A7" s="32"/>
       <c r="B7" s="32"/>
       <c r="C7" s="44"/>
@@ -12276,7 +12299,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
@@ -12289,7 +12312,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -12302,7 +12325,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="42"/>
@@ -12315,7 +12338,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="42"/>
@@ -12328,7 +12351,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="42"/>
@@ -12341,7 +12364,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -12354,7 +12377,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -12367,7 +12390,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -12380,7 +12403,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -12393,7 +12416,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -12406,7 +12429,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="32"/>
@@ -12419,7 +12442,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -12432,7 +12455,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -12445,7 +12468,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -12458,7 +12481,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -12471,7 +12494,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -12484,7 +12507,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -12497,7 +12520,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -12510,7 +12533,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -12523,7 +12546,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -12536,7 +12559,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -12549,7 +12572,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -12569,12 +12592,12 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -12590,7 +12613,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -12625,7 +12648,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>198</v>
       </c>
@@ -12654,7 +12677,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>199</v>
       </c>
@@ -12683,7 +12706,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>200</v>
       </c>
@@ -12712,7 +12735,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="142.5" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>201</v>
       </c>
@@ -12741,7 +12764,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>202</v>
       </c>
@@ -12770,7 +12793,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>215</v>
       </c>
@@ -12799,7 +12822,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A8" s="32"/>
       <c r="B8" s="32"/>
       <c r="C8" s="32"/>
@@ -12812,7 +12835,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1">
       <c r="A9" s="32"/>
       <c r="B9" s="32"/>
       <c r="C9" s="32"/>
@@ -12825,7 +12848,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A10" s="32"/>
       <c r="B10" s="32"/>
       <c r="C10" s="42"/>
@@ -12838,7 +12861,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="42"/>
@@ -12851,7 +12874,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="42"/>
@@ -12864,7 +12887,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -12877,7 +12900,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -12890,7 +12913,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -12903,7 +12926,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -12916,7 +12939,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -12929,7 +12952,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="32"/>
@@ -12942,7 +12965,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -12955,7 +12978,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -12968,7 +12991,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -12981,7 +13004,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -12994,7 +13017,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -13007,7 +13030,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -13020,7 +13043,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -13033,7 +13056,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -13046,7 +13069,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -13059,7 +13082,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -13072,7 +13095,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>
@@ -13092,14 +13115,14 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView zoomScale="40" zoomScaleNormal="40" workbookViewId="0">
       <selection activeCell="G4" sqref="G4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
+  <sheetFormatPr defaultRowHeight="90.75"/>
   <cols>
     <col min="1" max="1" width="22.85546875" style="34" customWidth="1"/>
     <col min="2" max="2" width="27.5703125" style="34" customWidth="1"/>
@@ -13115,7 +13138,7 @@
     <col min="12" max="16384" width="9.140625" style="34"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="22.5" customHeight="1">
       <c r="A1" s="38" t="s">
         <v>30</v>
       </c>
@@ -13150,7 +13173,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1">
       <c r="A2" s="32" t="s">
         <v>224</v>
       </c>
@@ -13179,7 +13202,7 @@
       <c r="J2" s="32"/>
       <c r="K2" s="32"/>
     </row>
-    <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1">
       <c r="A3" s="32" t="s">
         <v>225</v>
       </c>
@@ -13208,7 +13231,7 @@
       <c r="J3" s="32"/>
       <c r="K3" s="32"/>
     </row>
-    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1">
       <c r="A4" s="32" t="s">
         <v>226</v>
       </c>
@@ -13237,7 +13260,7 @@
       <c r="J4" s="32"/>
       <c r="K4" s="32"/>
     </row>
-    <row r="5" spans="1:11" s="33" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" s="33" customFormat="1" ht="142.5" customHeight="1">
       <c r="A5" s="32" t="s">
         <v>227</v>
       </c>
@@ -13266,7 +13289,7 @@
       <c r="J5" s="32"/>
       <c r="K5" s="32"/>
     </row>
-    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1">
       <c r="A6" s="32" t="s">
         <v>228</v>
       </c>
@@ -13295,7 +13318,7 @@
       <c r="J6" s="32"/>
       <c r="K6" s="32"/>
     </row>
-    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A7" s="32" t="s">
         <v>229</v>
       </c>
@@ -13324,7 +13347,7 @@
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
-    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A8" s="32" t="s">
         <v>246</v>
       </c>
@@ -13353,7 +13376,7 @@
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
-    <row r="9" spans="1:11" s="33" customFormat="1" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" s="33" customFormat="1" ht="127.5" customHeight="1">
       <c r="A9" s="32" t="s">
         <v>247</v>
       </c>
@@ -13382,7 +13405,7 @@
       <c r="J9" s="32"/>
       <c r="K9" s="32"/>
     </row>
-    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A10" s="32" t="s">
         <v>248</v>
       </c>
@@ -13411,7 +13434,7 @@
       <c r="J10" s="32"/>
       <c r="K10" s="32"/>
     </row>
-    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1">
       <c r="A11" s="32"/>
       <c r="B11" s="32"/>
       <c r="C11" s="42"/>
@@ -13424,7 +13447,7 @@
       <c r="J11" s="32"/>
       <c r="K11" s="32"/>
     </row>
-    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1">
       <c r="A12" s="32"/>
       <c r="B12" s="32"/>
       <c r="C12" s="42"/>
@@ -13437,7 +13460,7 @@
       <c r="J12" s="32"/>
       <c r="K12" s="32"/>
     </row>
-    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A13" s="32"/>
       <c r="B13" s="32"/>
       <c r="C13" s="32"/>
@@ -13450,7 +13473,7 @@
       <c r="J13" s="32"/>
       <c r="K13" s="32"/>
     </row>
-    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A14" s="32"/>
       <c r="B14" s="32"/>
       <c r="C14" s="32"/>
@@ -13463,7 +13486,7 @@
       <c r="J14" s="32"/>
       <c r="K14" s="32"/>
     </row>
-    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" s="33" customFormat="1" ht="184.5" customHeight="1">
       <c r="A15" s="32"/>
       <c r="B15" s="32"/>
       <c r="C15" s="32"/>
@@ -13476,7 +13499,7 @@
       <c r="J15" s="32"/>
       <c r="K15" s="32"/>
     </row>
-    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1">
       <c r="A16" s="32"/>
       <c r="B16" s="32"/>
       <c r="C16" s="32"/>
@@ -13489,7 +13512,7 @@
       <c r="J16" s="32"/>
       <c r="K16" s="32"/>
     </row>
-    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A17" s="32"/>
       <c r="B17" s="32"/>
       <c r="C17" s="32"/>
@@ -13502,7 +13525,7 @@
       <c r="J17" s="32"/>
       <c r="K17" s="32"/>
     </row>
-    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A18" s="42"/>
       <c r="B18" s="42"/>
       <c r="C18" s="32"/>
@@ -13515,7 +13538,7 @@
       <c r="J18" s="32"/>
       <c r="K18" s="32"/>
     </row>
-    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A19" s="42"/>
       <c r="B19" s="42"/>
       <c r="C19" s="32"/>
@@ -13528,7 +13551,7 @@
       <c r="J19" s="32"/>
       <c r="K19" s="32"/>
     </row>
-    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A20" s="42"/>
       <c r="B20" s="42"/>
       <c r="C20" s="32"/>
@@ -13541,7 +13564,7 @@
       <c r="J20" s="32"/>
       <c r="K20" s="32"/>
     </row>
-    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A21" s="32"/>
       <c r="B21" s="32"/>
       <c r="C21" s="32"/>
@@ -13554,7 +13577,7 @@
       <c r="J21" s="32"/>
       <c r="K21" s="32"/>
     </row>
-    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A22" s="32"/>
       <c r="B22" s="32"/>
       <c r="C22" s="32"/>
@@ -13567,7 +13590,7 @@
       <c r="J22" s="32"/>
       <c r="K22" s="32"/>
     </row>
-    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A23" s="32"/>
       <c r="B23" s="32"/>
       <c r="C23" s="32"/>
@@ -13580,7 +13603,7 @@
       <c r="J23" s="32"/>
       <c r="K23" s="32"/>
     </row>
-    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A24" s="32"/>
       <c r="B24" s="32"/>
       <c r="C24" s="32"/>
@@ -13593,7 +13616,7 @@
       <c r="J24" s="32"/>
       <c r="K24" s="32"/>
     </row>
-    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A25" s="32"/>
       <c r="B25" s="32"/>
       <c r="C25" s="32"/>
@@ -13606,7 +13629,7 @@
       <c r="J25" s="32"/>
       <c r="K25" s="32"/>
     </row>
-    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A26" s="32"/>
       <c r="B26" s="32"/>
       <c r="C26" s="32"/>
@@ -13619,7 +13642,7 @@
       <c r="J26" s="32"/>
       <c r="K26" s="32"/>
     </row>
-    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A27" s="32"/>
       <c r="B27" s="32"/>
       <c r="C27" s="32"/>
@@ -13632,7 +13655,7 @@
       <c r="J27" s="32"/>
       <c r="K27" s="32"/>
     </row>
-    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A28" s="32"/>
       <c r="B28" s="32"/>
       <c r="C28" s="32"/>
@@ -13645,7 +13668,7 @@
       <c r="J28" s="32"/>
       <c r="K28" s="32"/>
     </row>
-    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1">
       <c r="A29" s="32"/>
       <c r="B29" s="32"/>
       <c r="C29" s="32"/>

</xml_diff>

<commit_message>
17.11.2023 Product Display Testing.
</commit_message>
<xml_diff>
--- a/src/test/manual/Swag Labs-Test Scenarios.xlsx
+++ b/src/test/manual/Swag Labs-Test Scenarios.xlsx
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="963" uniqueCount="461">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="989" uniqueCount="469">
   <si>
     <t>Project Name</t>
   </si>
@@ -2369,29 +2369,6 @@
     <t xml:space="preserve">1. Open the Application URL, "https://www.saucedemo.com", in any  suported web Browser                                     2. User is logged in                                            3. Entered to the product page                    </t>
   </si>
   <si>
-    <t>1. Compare the actual price with expected result</t>
-  </si>
-  <si>
-    <t>The Price should be $29.99</t>
-  </si>
-  <si>
-    <r>
-      <t xml:space="preserve">The title should be </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="14"/>
-        <color theme="1"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <charset val="204"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>"Sauce Labs Backpack"</t>
-    </r>
-  </si>
-  <si>
     <r>
       <t xml:space="preserve">Validate the products </t>
     </r>
@@ -2702,9 +2679,6 @@
       </rPr>
       <t xml:space="preserve"> button                                                                                                          </t>
     </r>
-  </si>
-  <si>
-    <t>1. Compare the product title with expected result</t>
   </si>
   <si>
     <t>TC_AC_01</t>
@@ -5760,13 +5734,61 @@
   </si>
   <si>
     <t>Placeholder exist: true</t>
+  </si>
+  <si>
+    <t>The title should be same as with entered.</t>
+  </si>
+  <si>
+    <t>From Home page: 
+Sauce Labs Backpack
+From product display page: 
+Sauce Labs Backpack</t>
+  </si>
+  <si>
+    <t>1. Click on first product</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL, "https://www.saucedemo.com", in any  suported web Browser                                     2. User is logged in                                                            </t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Open the Application URL, "https://www.saucedemo.com", in any  suported web Browser                                                    </t>
+  </si>
+  <si>
+    <t>1. Click on last product</t>
+  </si>
+  <si>
+    <t>From Home page: 
+Test.allTheThings() T-Shirt (Red)
+From product display page: 
+Test.allTheThings() T-Shirt (Red)</t>
+  </si>
+  <si>
+    <t>The price should be same as with entered.</t>
+  </si>
+  <si>
+    <t>TC_PD_06</t>
+  </si>
+  <si>
+    <t>TC_PD_07</t>
+  </si>
+  <si>
+    <t>From Home page: 
+$29.99
+From product display page: 
+$29.99</t>
+  </si>
+  <si>
+    <t>From Home page: 
+$15.99
+From product display page: 
+$15.99</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="128" x14ac:knownFonts="1">
+  <fonts count="140" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -6144,66 +6166,6 @@
     </font>
     <font>
       <sz val="72"/>
-      <color indexed="58"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="72"/>
-      <color indexed="58"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="72"/>
-      <color indexed="58"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="72"/>
-      <color indexed="58"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="14"/>
-      <color indexed="12"/>
-      <name val="Calibri"/>
-    </font>
-    <font>
-      <sz val="72"/>
       <color indexed="16"/>
       <name val="Calibri"/>
     </font>
@@ -6472,8 +6434,128 @@
       <color indexed="12"/>
       <name val="Calibri"/>
     </font>
+    <font>
+      <sz val="72"/>
+      <color indexed="58"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color indexed="58"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color indexed="58"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color indexed="58"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color indexed="58"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color indexed="58"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color indexed="58"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="72"/>
+      <color indexed="58"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color indexed="12"/>
+      <name val="Calibri"/>
+    </font>
   </fonts>
-  <fills count="39">
+  <fills count="43">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -6535,26 +6617,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor indexed="10"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor indexed="42"/>
       </patternFill>
     </fill>
     <fill>
@@ -6667,8 +6729,48 @@
         <fgColor indexed="42"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor indexed="42"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="43">
+  <borders count="47">
     <border>
       <left/>
       <right/>
@@ -7288,6 +7390,66 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="8"/>
+      </left>
+      <right style="medium">
+        <color indexed="8"/>
+      </right>
+      <top style="medium">
+        <color indexed="8"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="8"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -7295,7 +7457,7 @@
     <xf numFmtId="0" fontId="22" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="24" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="163">
+  <cellXfs count="175">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -7768,6 +7930,42 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="127" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="128" fillId="39" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="129" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="130" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="131" fillId="40" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="132" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="133" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="134" fillId="41" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="135" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="136" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="137" fillId="42" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="138" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="139" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -8072,7 +8270,7 @@
   <dimension ref="A1:E43"/>
   <sheetViews>
     <sheetView topLeftCell="B10" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.25"/>
@@ -8096,10 +8294,10 @@
       <c r="A2" s="25" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="160" t="s">
+      <c r="B2" s="172" t="s">
         <v>29</v>
       </c>
-      <c r="C2" s="161"/>
+      <c r="C2" s="173"/>
       <c r="D2" s="2"/>
       <c r="E2" s="2"/>
     </row>
@@ -8129,10 +8327,10 @@
       <c r="A5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="B5" s="162" t="s">
+      <c r="B5" s="174" t="s">
         <v>23</v>
       </c>
-      <c r="C5" s="161"/>
+      <c r="C5" s="173"/>
       <c r="D5" s="2"/>
       <c r="E5" s="2"/>
     </row>
@@ -8247,7 +8445,7 @@
         <v>1</v>
       </c>
       <c r="D15" s="7">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E15" s="2"/>
     </row>
@@ -8271,7 +8469,7 @@
         <v>14</v>
       </c>
       <c r="B17" s="16" t="s">
-        <v>194</v>
+        <v>190</v>
       </c>
       <c r="C17" s="6">
         <v>1</v>
@@ -8292,7 +8490,7 @@
         <v>1</v>
       </c>
       <c r="D18" s="8" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="E18" s="2"/>
     </row>
@@ -8316,7 +8514,7 @@
         <v>17</v>
       </c>
       <c r="B20" s="16" t="s">
-        <v>360</v>
+        <v>356</v>
       </c>
       <c r="C20" s="6">
         <v>1</v>
@@ -8331,7 +8529,7 @@
         <v>18</v>
       </c>
       <c r="B21" s="16" t="s">
-        <v>361</v>
+        <v>357</v>
       </c>
       <c r="C21" s="9">
         <v>1</v>
@@ -8343,7 +8541,7 @@
     </row>
     <row r="22" spans="1:5" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A22" s="12" t="s">
-        <v>364</v>
+        <v>360</v>
       </c>
       <c r="B22" s="17" t="s">
         <v>21</v>
@@ -8575,25 +8773,25 @@
     </row>
     <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="47">
@@ -8604,25 +8802,25 @@
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>269</v>
+        <v>265</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="47">
@@ -8633,25 +8831,25 @@
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="47">
@@ -8662,25 +8860,25 @@
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>262</v>
+        <v>258</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>305</v>
+        <v>301</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="47">
@@ -8691,25 +8889,25 @@
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="47">
@@ -8720,25 +8918,25 @@
     </row>
     <row r="7" spans="1:11" s="33" customFormat="1" ht="117" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="F7" s="37" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H7" s="32"/>
       <c r="I7" s="47">
@@ -8749,25 +8947,25 @@
     </row>
     <row r="8" spans="1:11" s="33" customFormat="1" ht="107.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="F8" s="37" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="47">
@@ -8778,25 +8976,25 @@
     </row>
     <row r="9" spans="1:11" s="33" customFormat="1" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>299</v>
+        <v>295</v>
       </c>
       <c r="H9" s="32"/>
       <c r="I9" s="47">
@@ -8807,25 +9005,25 @@
     </row>
     <row r="10" spans="1:11" s="33" customFormat="1" ht="124.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>301</v>
+        <v>297</v>
       </c>
       <c r="H10" s="32"/>
       <c r="I10" s="47">
@@ -8836,25 +9034,25 @@
     </row>
     <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>300</v>
+        <v>296</v>
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="47">
@@ -8865,25 +9063,25 @@
     </row>
     <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="B12" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C12" s="42" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="D12" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E12" s="35" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="F12" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="H12" s="32"/>
       <c r="I12" s="47">
@@ -8894,25 +9092,25 @@
     </row>
     <row r="13" spans="1:11" s="33" customFormat="1" ht="213.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="32" t="s">
+        <v>294</v>
+      </c>
+      <c r="B13" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="C13" s="44" t="s">
+        <v>293</v>
+      </c>
+      <c r="D13" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="E13" s="35" t="s">
         <v>298</v>
       </c>
-      <c r="B13" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="C13" s="44" t="s">
-        <v>297</v>
-      </c>
-      <c r="D13" s="41" t="s">
-        <v>257</v>
-      </c>
-      <c r="E13" s="35" t="s">
-        <v>302</v>
-      </c>
       <c r="F13" s="37" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G13" s="35" t="s">
-        <v>304</v>
+        <v>300</v>
       </c>
       <c r="H13" s="32"/>
       <c r="I13" s="47">
@@ -8923,25 +9121,25 @@
     </row>
     <row r="14" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="32" t="s">
-        <v>306</v>
+        <v>302</v>
       </c>
       <c r="B14" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C14" s="44" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="D14" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E14" s="35" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="F14" s="37" t="s">
-        <v>303</v>
+        <v>299</v>
       </c>
       <c r="G14" s="35" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H14" s="32"/>
       <c r="I14" s="47">
@@ -8952,25 +9150,25 @@
     </row>
     <row r="15" spans="1:11" s="33" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
+        <v>303</v>
+      </c>
+      <c r="B15" s="32" t="s">
+        <v>263</v>
+      </c>
+      <c r="C15" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="D15" s="41" t="s">
+        <v>253</v>
+      </c>
+      <c r="E15" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="F15" s="37" t="s">
+        <v>306</v>
+      </c>
+      <c r="G15" s="35" t="s">
         <v>307</v>
-      </c>
-      <c r="B15" s="32" t="s">
-        <v>267</v>
-      </c>
-      <c r="C15" s="44" t="s">
-        <v>313</v>
-      </c>
-      <c r="D15" s="41" t="s">
-        <v>257</v>
-      </c>
-      <c r="E15" s="35" t="s">
-        <v>308</v>
-      </c>
-      <c r="F15" s="37" t="s">
-        <v>310</v>
-      </c>
-      <c r="G15" s="35" t="s">
-        <v>311</v>
       </c>
       <c r="H15" s="32"/>
       <c r="I15" s="47">
@@ -8981,25 +9179,25 @@
     </row>
     <row r="16" spans="1:11" s="33" customFormat="1" ht="151.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A16" s="32" t="s">
-        <v>319</v>
+        <v>315</v>
       </c>
       <c r="B16" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C16" s="44" t="s">
-        <v>315</v>
+        <v>311</v>
       </c>
       <c r="D16" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E16" s="35" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F16" s="37" t="s">
-        <v>314</v>
+        <v>310</v>
       </c>
       <c r="G16" s="35" t="s">
-        <v>311</v>
+        <v>307</v>
       </c>
       <c r="H16" s="32"/>
       <c r="I16" s="47">
@@ -9010,25 +9208,25 @@
     </row>
     <row r="17" spans="1:11" s="33" customFormat="1" ht="153.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>320</v>
+        <v>316</v>
       </c>
       <c r="B17" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C17" s="44" t="s">
-        <v>322</v>
+        <v>318</v>
       </c>
       <c r="D17" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E17" s="35" t="s">
+        <v>304</v>
+      </c>
+      <c r="F17" s="37" t="s">
         <v>308</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="G17" s="35" t="s">
         <v>312</v>
-      </c>
-      <c r="G17" s="35" t="s">
-        <v>316</v>
       </c>
       <c r="H17" s="32"/>
       <c r="I17" s="47">
@@ -9039,25 +9237,25 @@
     </row>
     <row r="18" spans="1:11" s="33" customFormat="1" ht="155.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>321</v>
+        <v>317</v>
       </c>
       <c r="B18" s="32" t="s">
-        <v>267</v>
+        <v>263</v>
       </c>
       <c r="C18" s="44" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="D18" s="41" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="E18" s="35" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="F18" s="37" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="G18" s="35" t="s">
-        <v>317</v>
+        <v>313</v>
       </c>
       <c r="H18" s="32"/>
       <c r="I18" s="47">
@@ -9276,25 +9474,25 @@
     </row>
     <row r="2" spans="1:11" s="33" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>325</v>
+        <v>321</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>336</v>
+        <v>332</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>342</v>
+        <v>338</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F2" s="37" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>335</v>
+        <v>331</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="47">
@@ -9305,25 +9503,25 @@
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="135" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>326</v>
+        <v>322</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C3" s="44" t="s">
+        <v>333</v>
+      </c>
+      <c r="D3" s="41" t="s">
         <v>337</v>
       </c>
-      <c r="D3" s="41" t="s">
-        <v>341</v>
-      </c>
       <c r="E3" s="35" t="s">
-        <v>338</v>
+        <v>334</v>
       </c>
       <c r="F3" s="37" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>339</v>
+        <v>335</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="47">
@@ -9334,25 +9532,25 @@
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>327</v>
+        <v>323</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>340</v>
+        <v>336</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>345</v>
+        <v>341</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>343</v>
+        <v>339</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>344</v>
+        <v>340</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="47">
@@ -9363,25 +9561,25 @@
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="157.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>328</v>
+        <v>324</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>347</v>
+        <v>343</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>348</v>
+        <v>344</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>349</v>
+        <v>345</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="47">
@@ -9392,25 +9590,25 @@
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>329</v>
+        <v>325</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>350</v>
+        <v>346</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="47">
@@ -9421,25 +9619,25 @@
     </row>
     <row r="7" spans="1:11" s="33" customFormat="1" ht="150" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>330</v>
+        <v>326</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>353</v>
+        <v>349</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F7" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="H7" s="32"/>
       <c r="I7" s="47">
@@ -9450,25 +9648,25 @@
     </row>
     <row r="8" spans="1:11" s="33" customFormat="1" ht="162.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>331</v>
+        <v>327</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>356</v>
+        <v>352</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E8" s="35" t="s">
-        <v>362</v>
+        <v>358</v>
       </c>
       <c r="F8" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>363</v>
+        <v>359</v>
       </c>
       <c r="H8" s="32"/>
       <c r="I8" s="47">
@@ -9479,25 +9677,25 @@
     </row>
     <row r="9" spans="1:11" s="33" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>332</v>
+        <v>328</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C9" s="44" t="s">
-        <v>358</v>
+        <v>354</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>351</v>
+        <v>347</v>
       </c>
       <c r="F9" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>352</v>
+        <v>348</v>
       </c>
       <c r="H9" s="32"/>
       <c r="I9" s="47">
@@ -9508,25 +9706,25 @@
     </row>
     <row r="10" spans="1:11" s="33" customFormat="1" ht="156.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>333</v>
+        <v>329</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>359</v>
+        <v>355</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>354</v>
+        <v>350</v>
       </c>
       <c r="F10" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="H10" s="32"/>
       <c r="I10" s="47">
@@ -9537,25 +9735,25 @@
     </row>
     <row r="11" spans="1:11" s="33" customFormat="1" ht="159.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
-        <v>334</v>
+        <v>330</v>
       </c>
       <c r="B11" s="32" t="s">
-        <v>324</v>
+        <v>320</v>
       </c>
       <c r="C11" s="44" t="s">
-        <v>365</v>
+        <v>361</v>
       </c>
       <c r="D11" s="41" t="s">
-        <v>357</v>
+        <v>353</v>
       </c>
       <c r="E11" s="35" t="s">
-        <v>366</v>
+        <v>362</v>
       </c>
       <c r="F11" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>367</v>
+        <v>363</v>
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="47">
@@ -9865,25 +10063,25 @@
     </row>
     <row r="2" spans="1:11" s="33" customFormat="1" ht="153" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>369</v>
+        <v>365</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>346</v>
+        <v>342</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>368</v>
+        <v>364</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>355</v>
+        <v>351</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="47">
@@ -9894,23 +10092,23 @@
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="177" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="B3" s="32" t="s">
+        <v>367</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>371</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>375</v>
-      </c>
       <c r="D3" s="41" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="F3" s="37"/>
       <c r="G3" s="35" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="47">
@@ -10323,25 +10521,25 @@
     </row>
     <row r="2" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C2" s="32" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="47">
@@ -10352,25 +10550,25 @@
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B3" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C3" s="32" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="47">
@@ -10381,25 +10579,25 @@
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>223</v>
+        <v>219</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C4" s="32" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="47">
@@ -10410,25 +10608,25 @@
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B5" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="C5" s="32" t="s">
         <v>377</v>
       </c>
-      <c r="C5" s="32" t="s">
-        <v>381</v>
-      </c>
       <c r="D5" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="47">
@@ -10439,19 +10637,19 @@
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E6" s="51" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>58</v>
@@ -10466,25 +10664,25 @@
     </row>
     <row r="7" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C7" s="32" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="F7" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="H7" s="32"/>
       <c r="I7" s="47">
@@ -10495,19 +10693,19 @@
     </row>
     <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="D8" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E8" s="52" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="F8" s="37" t="s">
         <v>58</v>
@@ -10522,19 +10720,19 @@
     </row>
     <row r="9" spans="1:11" s="33" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
-        <v>244</v>
+        <v>240</v>
       </c>
       <c r="B9" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="D9" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E9" s="53" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="F9" s="37" t="s">
         <v>58</v>
@@ -10549,25 +10747,25 @@
     </row>
     <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="C10" s="42" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E10" s="41" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="F10" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G10" s="41" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="H10" s="32"/>
       <c r="I10" s="47"/>
@@ -10576,25 +10774,25 @@
     </row>
     <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="32" t="s">
+        <v>394</v>
+      </c>
+      <c r="B11" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="C11" s="42" t="s">
         <v>398</v>
       </c>
-      <c r="B11" s="32" t="s">
-        <v>377</v>
-      </c>
-      <c r="C11" s="42" t="s">
-        <v>402</v>
-      </c>
       <c r="D11" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E11" s="41" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="F11" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G11" s="41" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="H11" s="32"/>
       <c r="I11" s="47"/>
@@ -10603,25 +10801,25 @@
     </row>
     <row r="12" spans="1:11" s="33" customFormat="1" ht="140.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="32" t="s">
+        <v>395</v>
+      </c>
+      <c r="B12" s="32" t="s">
+        <v>373</v>
+      </c>
+      <c r="C12" s="42" t="s">
         <v>399</v>
       </c>
-      <c r="B12" s="32" t="s">
-        <v>377</v>
-      </c>
-      <c r="C12" s="42" t="s">
-        <v>403</v>
-      </c>
       <c r="D12" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E12" s="41" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="F12" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G12" s="41" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="H12" s="32"/>
       <c r="I12" s="47"/>
@@ -10864,7 +11062,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K29"/>
   <sheetViews>
-    <sheetView zoomScale="10" zoomScaleNormal="10" workbookViewId="0">
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="J22" sqref="J22"/>
     </sheetView>
   </sheetViews>
@@ -10941,17 +11139,17 @@
       <c r="G2" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="H2" s="150" t="s">
-        <v>457</v>
+      <c r="H2" s="138" t="s">
+        <v>453</v>
       </c>
       <c r="I2" s="47">
         <v>0</v>
       </c>
-      <c r="J2" s="148" t="s">
-        <v>434</v>
-      </c>
-      <c r="K2" s="149" t="s">
-        <v>436</v>
+      <c r="J2" s="136" t="s">
+        <v>430</v>
+      </c>
+      <c r="K2" s="137" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -10974,19 +11172,19 @@
         <v>51</v>
       </c>
       <c r="G3" s="54" t="s">
-        <v>409</v>
-      </c>
-      <c r="H3" s="117" t="s">
-        <v>455</v>
+        <v>405</v>
+      </c>
+      <c r="H3" s="105" t="s">
+        <v>451</v>
       </c>
       <c r="I3" s="47">
         <v>0</v>
       </c>
-      <c r="J3" s="115" t="s">
-        <v>434</v>
-      </c>
-      <c r="K3" s="116" t="s">
-        <v>436</v>
+      <c r="J3" s="103" t="s">
+        <v>430</v>
+      </c>
+      <c r="K3" s="104" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11009,19 +11207,19 @@
         <v>49</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>412</v>
-      </c>
-      <c r="H4" s="120" t="s">
-        <v>455</v>
+        <v>408</v>
+      </c>
+      <c r="H4" s="108" t="s">
+        <v>451</v>
       </c>
       <c r="I4" s="47">
         <v>0</v>
       </c>
-      <c r="J4" s="118" t="s">
-        <v>434</v>
-      </c>
-      <c r="K4" s="119" t="s">
-        <v>436</v>
+      <c r="J4" s="106" t="s">
+        <v>430</v>
+      </c>
+      <c r="K4" s="107" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11044,19 +11242,19 @@
         <v>52</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>413</v>
-      </c>
-      <c r="H5" s="153" t="s">
-        <v>455</v>
+        <v>409</v>
+      </c>
+      <c r="H5" s="141" t="s">
+        <v>451</v>
       </c>
       <c r="I5" s="47">
         <v>0</v>
       </c>
-      <c r="J5" s="151" t="s">
-        <v>434</v>
-      </c>
-      <c r="K5" s="152" t="s">
-        <v>436</v>
+      <c r="J5" s="139" t="s">
+        <v>430</v>
+      </c>
+      <c r="K5" s="140" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11079,19 +11277,19 @@
         <v>58</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>414</v>
-      </c>
-      <c r="H6" s="123" t="s">
-        <v>455</v>
+        <v>410</v>
+      </c>
+      <c r="H6" s="111" t="s">
+        <v>451</v>
       </c>
       <c r="I6" s="47">
         <v>0</v>
       </c>
-      <c r="J6" s="121" t="s">
-        <v>434</v>
-      </c>
-      <c r="K6" s="122" t="s">
-        <v>436</v>
+      <c r="J6" s="109" t="s">
+        <v>430</v>
+      </c>
+      <c r="K6" s="110" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11114,19 +11312,19 @@
         <v>70</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>415</v>
-      </c>
-      <c r="H7" s="156" t="s">
-        <v>455</v>
+        <v>411</v>
+      </c>
+      <c r="H7" s="144" t="s">
+        <v>451</v>
       </c>
       <c r="I7" s="47">
         <v>0</v>
       </c>
-      <c r="J7" s="154" t="s">
-        <v>434</v>
-      </c>
-      <c r="K7" s="155" t="s">
-        <v>436</v>
+      <c r="J7" s="142" t="s">
+        <v>430</v>
+      </c>
+      <c r="K7" s="143" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11146,22 +11344,22 @@
         <v>69</v>
       </c>
       <c r="F8" s="40" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>410</v>
-      </c>
-      <c r="H8" s="159" t="s">
-        <v>455</v>
+        <v>406</v>
+      </c>
+      <c r="H8" s="147" t="s">
+        <v>451</v>
       </c>
       <c r="I8" s="47">
         <v>0</v>
       </c>
-      <c r="J8" s="157" t="s">
-        <v>434</v>
-      </c>
-      <c r="K8" s="158" t="s">
-        <v>436</v>
+      <c r="J8" s="145" t="s">
+        <v>430</v>
+      </c>
+      <c r="K8" s="146" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="33" customFormat="1" ht="105.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11172,31 +11370,31 @@
         <v>41</v>
       </c>
       <c r="C9" s="32" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="D9" s="35" t="s">
         <v>77</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="F9" s="37" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>412</v>
-      </c>
-      <c r="H9" s="135" t="s">
-        <v>455</v>
+        <v>408</v>
+      </c>
+      <c r="H9" s="123" t="s">
+        <v>451</v>
       </c>
       <c r="I9" s="47">
         <v>0</v>
       </c>
-      <c r="J9" s="133" t="s">
-        <v>434</v>
-      </c>
-      <c r="K9" s="134" t="s">
-        <v>436</v>
+      <c r="J9" s="121" t="s">
+        <v>430</v>
+      </c>
+      <c r="K9" s="122" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="10" spans="1:11" s="33" customFormat="1" ht="101.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11207,31 +11405,31 @@
         <v>41</v>
       </c>
       <c r="C10" s="32" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="D10" s="35" t="s">
         <v>77</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="F10" s="37" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>412</v>
-      </c>
-      <c r="H10" s="144" t="s">
-        <v>455</v>
+        <v>408</v>
+      </c>
+      <c r="H10" s="132" t="s">
+        <v>451</v>
       </c>
       <c r="I10" s="47">
         <v>0</v>
       </c>
-      <c r="J10" s="142" t="s">
-        <v>434</v>
-      </c>
-      <c r="K10" s="143" t="s">
-        <v>436</v>
+      <c r="J10" s="130" t="s">
+        <v>430</v>
+      </c>
+      <c r="K10" s="131" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="11" spans="1:11" s="33" customFormat="1" ht="122.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -11242,7 +11440,7 @@
         <v>41</v>
       </c>
       <c r="C11" s="32" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="D11" s="35" t="s">
         <v>77</v>
@@ -11251,22 +11449,22 @@
         <v>43</v>
       </c>
       <c r="F11" s="37" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="G11" s="35" t="s">
-        <v>412</v>
-      </c>
-      <c r="H11" s="138" t="s">
-        <v>455</v>
+        <v>408</v>
+      </c>
+      <c r="H11" s="126" t="s">
+        <v>451</v>
       </c>
       <c r="I11" s="47">
         <v>0</v>
       </c>
-      <c r="J11" s="136" t="s">
-        <v>434</v>
-      </c>
-      <c r="K11" s="137" t="s">
-        <v>436</v>
+      <c r="J11" s="124" t="s">
+        <v>430</v>
+      </c>
+      <c r="K11" s="125" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="12" spans="1:11" s="33" customFormat="1" ht="112.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11277,7 +11475,7 @@
         <v>41</v>
       </c>
       <c r="C12" s="32" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="D12" s="35" t="s">
         <v>77</v>
@@ -11286,22 +11484,22 @@
         <v>43</v>
       </c>
       <c r="F12" s="37" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="G12" s="35" t="s">
-        <v>412</v>
-      </c>
-      <c r="H12" s="147" t="s">
-        <v>455</v>
+        <v>408</v>
+      </c>
+      <c r="H12" s="135" t="s">
+        <v>451</v>
       </c>
       <c r="I12" s="47">
         <v>0</v>
       </c>
-      <c r="J12" s="145" t="s">
-        <v>434</v>
-      </c>
-      <c r="K12" s="146" t="s">
-        <v>436</v>
+      <c r="J12" s="133" t="s">
+        <v>430</v>
+      </c>
+      <c r="K12" s="134" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="13" spans="1:11" s="33" customFormat="1" ht="175.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11326,17 +11524,17 @@
       <c r="G13" s="35" t="s">
         <v>66</v>
       </c>
-      <c r="H13" s="126" t="s">
-        <v>457</v>
+      <c r="H13" s="114" t="s">
+        <v>453</v>
       </c>
       <c r="I13" s="47">
         <v>2</v>
       </c>
-      <c r="J13" s="124" t="s">
-        <v>434</v>
-      </c>
-      <c r="K13" s="125" t="s">
-        <v>436</v>
+      <c r="J13" s="112" t="s">
+        <v>430</v>
+      </c>
+      <c r="K13" s="113" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="14" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11361,17 +11559,17 @@
       <c r="G14" s="41" t="s">
         <v>71</v>
       </c>
-      <c r="H14" s="141" t="s">
-        <v>460</v>
+      <c r="H14" s="129" t="s">
+        <v>456</v>
       </c>
       <c r="I14" s="47">
         <v>2</v>
       </c>
-      <c r="J14" s="139" t="s">
-        <v>434</v>
-      </c>
-      <c r="K14" s="140" t="s">
-        <v>436</v>
+      <c r="J14" s="127" t="s">
+        <v>430</v>
+      </c>
+      <c r="K14" s="128" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="15" spans="1:11" s="33" customFormat="1" ht="150.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11388,25 +11586,25 @@
         <v>77</v>
       </c>
       <c r="E15" s="41" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="F15" s="37" t="s">
         <v>44</v>
       </c>
       <c r="G15" s="41" t="s">
-        <v>430</v>
-      </c>
-      <c r="H15" s="129" t="s">
-        <v>455</v>
+        <v>426</v>
+      </c>
+      <c r="H15" s="117" t="s">
+        <v>451</v>
       </c>
       <c r="I15" s="47">
         <v>1</v>
       </c>
-      <c r="J15" s="127" t="s">
-        <v>434</v>
-      </c>
-      <c r="K15" s="128" t="s">
-        <v>436</v>
+      <c r="J15" s="115" t="s">
+        <v>430</v>
+      </c>
+      <c r="K15" s="116" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="16" spans="1:11" s="33" customFormat="1" ht="147.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -11417,7 +11615,7 @@
         <v>41</v>
       </c>
       <c r="C16" s="42" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D16" s="41" t="s">
         <v>77</v>
@@ -11429,24 +11627,24 @@
         <v>44</v>
       </c>
       <c r="G16" s="41" t="s">
-        <v>432</v>
-      </c>
-      <c r="H16" s="108" t="s">
-        <v>457</v>
+        <v>428</v>
+      </c>
+      <c r="H16" s="96" t="s">
+        <v>453</v>
       </c>
       <c r="I16" s="47">
         <v>1</v>
       </c>
-      <c r="J16" s="106" t="s">
-        <v>433</v>
-      </c>
-      <c r="K16" s="107" t="s">
-        <v>456</v>
+      <c r="J16" s="94" t="s">
+        <v>429</v>
+      </c>
+      <c r="K16" s="95" t="s">
+        <v>452</v>
       </c>
     </row>
     <row r="17" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A17" s="32" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="B17" s="42" t="s">
         <v>41</v>
@@ -11466,22 +11664,22 @@
       <c r="G17" s="35" t="s">
         <v>82</v>
       </c>
-      <c r="H17" s="132" t="s">
-        <v>459</v>
+      <c r="H17" s="120" t="s">
+        <v>455</v>
       </c>
       <c r="I17" s="47">
         <v>1</v>
       </c>
-      <c r="J17" s="130" t="s">
-        <v>434</v>
-      </c>
-      <c r="K17" s="131" t="s">
-        <v>436</v>
+      <c r="J17" s="118" t="s">
+        <v>430</v>
+      </c>
+      <c r="K17" s="119" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="18" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="32" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="B18" s="42" t="s">
         <v>41</v>
@@ -11501,28 +11699,28 @@
       <c r="G18" s="35" t="s">
         <v>86</v>
       </c>
-      <c r="H18" s="114" t="s">
-        <v>458</v>
+      <c r="H18" s="102" t="s">
+        <v>454</v>
       </c>
       <c r="I18" s="47">
         <v>1</v>
       </c>
-      <c r="J18" s="112" t="s">
-        <v>434</v>
-      </c>
-      <c r="K18" s="113" t="s">
-        <v>436</v>
+      <c r="J18" s="100" t="s">
+        <v>430</v>
+      </c>
+      <c r="K18" s="101" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="19" spans="1:11" s="33" customFormat="1" ht="168" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="32" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="B19" s="42" t="s">
         <v>41</v>
       </c>
       <c r="C19" s="32" t="s">
-        <v>453</v>
+        <v>449</v>
       </c>
       <c r="D19" s="41" t="s">
         <v>77</v>
@@ -11534,24 +11732,24 @@
         <v>91</v>
       </c>
       <c r="G19" s="35" t="s">
-        <v>454</v>
-      </c>
-      <c r="H19" s="111" t="s">
-        <v>455</v>
+        <v>450</v>
+      </c>
+      <c r="H19" s="99" t="s">
+        <v>451</v>
       </c>
       <c r="I19" s="47">
         <v>1</v>
       </c>
-      <c r="J19" s="109" t="s">
-        <v>434</v>
-      </c>
-      <c r="K19" s="110" t="s">
-        <v>436</v>
+      <c r="J19" s="97" t="s">
+        <v>430</v>
+      </c>
+      <c r="K19" s="98" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="20" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="32" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="B20" s="42" t="s">
         <v>41</v>
@@ -11782,17 +11980,17 @@
       <c r="G2" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="99" t="s">
-        <v>451</v>
+      <c r="H2" s="87" t="s">
+        <v>447</v>
       </c>
       <c r="I2" s="47">
         <v>0</v>
       </c>
-      <c r="J2" s="97" t="s">
-        <v>434</v>
-      </c>
-      <c r="K2" s="98" t="s">
-        <v>436</v>
+      <c r="J2" s="85" t="s">
+        <v>430</v>
+      </c>
+      <c r="K2" s="86" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="138" customHeight="1" x14ac:dyDescent="0.25">
@@ -11817,17 +12015,17 @@
       <c r="G3" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="H3" s="96" t="s">
-        <v>450</v>
+      <c r="H3" s="84" t="s">
+        <v>446</v>
       </c>
       <c r="I3" s="47">
         <v>1</v>
       </c>
-      <c r="J3" s="94" t="s">
-        <v>434</v>
-      </c>
-      <c r="K3" s="95" t="s">
-        <v>436</v>
+      <c r="J3" s="82" t="s">
+        <v>430</v>
+      </c>
+      <c r="K3" s="83" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="136.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11852,17 +12050,17 @@
       <c r="G4" s="35" t="s">
         <v>106</v>
       </c>
-      <c r="H4" s="105" t="s">
-        <v>452</v>
+      <c r="H4" s="93" t="s">
+        <v>448</v>
       </c>
       <c r="I4" s="50">
         <v>0</v>
       </c>
-      <c r="J4" s="103" t="s">
-        <v>434</v>
-      </c>
-      <c r="K4" s="104" t="s">
-        <v>436</v>
+      <c r="J4" s="91" t="s">
+        <v>430</v>
+      </c>
+      <c r="K4" s="92" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="156" customHeight="1" x14ac:dyDescent="0.25">
@@ -11887,17 +12085,17 @@
       <c r="G5" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="H5" s="102" t="s">
-        <v>452</v>
+      <c r="H5" s="90" t="s">
+        <v>448</v>
       </c>
       <c r="I5" s="50">
         <v>2</v>
       </c>
-      <c r="J5" s="100" t="s">
-        <v>434</v>
-      </c>
-      <c r="K5" s="101" t="s">
-        <v>436</v>
+      <c r="J5" s="88" t="s">
+        <v>430</v>
+      </c>
+      <c r="K5" s="89" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -11908,7 +12106,7 @@
         <v>97</v>
       </c>
       <c r="C6" s="32" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="D6" s="41" t="s">
         <v>108</v>
@@ -12315,17 +12513,17 @@
       <c r="G2" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="H2" s="84" t="s">
-        <v>448</v>
+      <c r="H2" s="150" t="s">
+        <v>444</v>
       </c>
       <c r="I2" s="47">
         <v>1</v>
       </c>
-      <c r="J2" s="82" t="s">
-        <v>434</v>
-      </c>
-      <c r="K2" s="83" t="s">
-        <v>436</v>
+      <c r="J2" s="148" t="s">
+        <v>430</v>
+      </c>
+      <c r="K2" s="149" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
@@ -12350,17 +12548,17 @@
       <c r="G3" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="H3" s="87" t="s">
-        <v>449</v>
+      <c r="H3" s="153" t="s">
+        <v>445</v>
       </c>
       <c r="I3" s="47">
         <v>1</v>
       </c>
-      <c r="J3" s="85" t="s">
-        <v>434</v>
-      </c>
-      <c r="K3" s="86" t="s">
-        <v>436</v>
+      <c r="J3" s="151" t="s">
+        <v>430</v>
+      </c>
+      <c r="K3" s="152" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12385,17 +12583,17 @@
       <c r="G4" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="H4" s="90" t="s">
-        <v>448</v>
+      <c r="H4" s="156" t="s">
+        <v>444</v>
       </c>
       <c r="I4" s="47">
         <v>0</v>
       </c>
-      <c r="J4" s="88" t="s">
-        <v>434</v>
-      </c>
-      <c r="K4" s="89" t="s">
-        <v>436</v>
+      <c r="J4" s="154" t="s">
+        <v>430</v>
+      </c>
+      <c r="K4" s="155" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="111.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -12420,17 +12618,17 @@
       <c r="G5" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="H5" s="93" t="s">
-        <v>449</v>
+      <c r="H5" s="159" t="s">
+        <v>445</v>
       </c>
       <c r="I5" s="47">
         <v>0</v>
       </c>
-      <c r="J5" s="91" t="s">
-        <v>434</v>
-      </c>
-      <c r="K5" s="92" t="s">
-        <v>436</v>
+      <c r="J5" s="157" t="s">
+        <v>430</v>
+      </c>
+      <c r="K5" s="158" t="s">
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12829,19 +13027,19 @@
         <v>58</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="H2" s="72" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="I2" s="47">
         <v>0</v>
       </c>
       <c r="J2" s="70" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K2" s="71" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
@@ -12867,16 +13065,16 @@
         <v>139</v>
       </c>
       <c r="H3" s="75" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="I3" s="60">
         <v>0</v>
       </c>
       <c r="J3" s="73" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K3" s="74" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -12902,16 +13100,16 @@
         <v>139</v>
       </c>
       <c r="H4" s="69" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="I4" s="47">
         <v>0</v>
       </c>
       <c r="J4" s="67" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K4" s="68" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12931,22 +13129,22 @@
         <v>145</v>
       </c>
       <c r="F5" s="37" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="G5" s="35" t="s">
         <v>139</v>
       </c>
       <c r="H5" s="66" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="I5" s="47">
         <v>0</v>
       </c>
       <c r="J5" s="64" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K5" s="65" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="139.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -12966,33 +13164,33 @@
         <v>149</v>
       </c>
       <c r="F6" s="37" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="G6" s="35" t="s">
         <v>139</v>
       </c>
       <c r="H6" s="63" t="s">
-        <v>445</v>
+        <v>441</v>
       </c>
       <c r="I6" s="47">
         <v>0</v>
       </c>
       <c r="J6" s="61" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K6" s="62" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="B7" s="32" t="s">
         <v>138</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="D7" s="41" t="s">
         <v>109</v>
@@ -13004,30 +13202,30 @@
         <v>58</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H7" s="81" t="s">
-        <v>447</v>
+        <v>443</v>
       </c>
       <c r="I7" s="47">
         <v>1</v>
       </c>
       <c r="J7" s="79" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="K7" s="80" t="s">
-        <v>444</v>
+        <v>440</v>
       </c>
     </row>
     <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>443</v>
+        <v>439</v>
       </c>
       <c r="B8" s="32" t="s">
         <v>138</v>
       </c>
       <c r="C8" s="44" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="D8" s="41" t="s">
         <v>109</v>
@@ -13039,19 +13237,19 @@
         <v>58</v>
       </c>
       <c r="G8" s="35" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="H8" s="78" t="s">
-        <v>446</v>
+        <v>442</v>
       </c>
       <c r="I8" s="47">
         <v>1</v>
       </c>
       <c r="J8" s="76" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="K8" s="77" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
     </row>
     <row r="9" spans="1:11" s="33" customFormat="1" ht="169.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -13338,7 +13536,7 @@
   <dimension ref="A1:K29"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H3" sqref="H3"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="90.75" x14ac:dyDescent="1.25"/>
@@ -13350,7 +13548,7 @@
     <col min="5" max="5" width="56.42578125" style="36" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="38.7109375" style="34" customWidth="1" collapsed="1"/>
     <col min="7" max="7" width="33.42578125" style="36" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="26.85546875" style="34" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="51.140625" style="34" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="17" style="48" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="19.5703125" style="34" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="46.7109375" style="34" customWidth="1" collapsed="1"/>
@@ -13400,26 +13598,32 @@
         <v>151</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>157</v>
+        <v>461</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>172</v>
+        <v>459</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="46" t="s">
-        <v>160</v>
-      </c>
-      <c r="H2" s="32"/>
+        <v>457</v>
+      </c>
+      <c r="H2" s="162" t="s">
+        <v>458</v>
+      </c>
       <c r="I2" s="47">
         <v>0</v>
       </c>
-      <c r="J2" s="32"/>
-      <c r="K2" s="32"/>
+      <c r="J2" s="160" t="s">
+        <v>430</v>
+      </c>
+      <c r="K2" s="161" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="99" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
@@ -13429,26 +13633,32 @@
         <v>151</v>
       </c>
       <c r="C3" s="44" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>157</v>
+        <v>460</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>158</v>
+        <v>462</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="G3" s="35" t="s">
-        <v>159</v>
-      </c>
-      <c r="H3" s="32"/>
+      <c r="G3" s="46" t="s">
+        <v>457</v>
+      </c>
+      <c r="H3" s="165" t="s">
+        <v>463</v>
+      </c>
       <c r="I3" s="47">
         <v>0</v>
       </c>
-      <c r="J3" s="32"/>
-      <c r="K3" s="32"/>
+      <c r="J3" s="163" t="s">
+        <v>430</v>
+      </c>
+      <c r="K3" s="164" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="92.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
@@ -13458,26 +13668,32 @@
         <v>151</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="D4" s="41" t="s">
         <v>157</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>163</v>
+        <v>459</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="G4" s="35" t="s">
-        <v>164</v>
-      </c>
-      <c r="H4" s="32"/>
+      <c r="G4" s="46" t="s">
+        <v>464</v>
+      </c>
+      <c r="H4" s="168" t="s">
+        <v>467</v>
+      </c>
       <c r="I4" s="47">
-        <v>1</v>
-      </c>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
+        <v>0</v>
+      </c>
+      <c r="J4" s="166" t="s">
+        <v>430</v>
+      </c>
+      <c r="K4" s="167" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="115.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
@@ -13487,26 +13703,32 @@
         <v>151</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>166</v>
+        <v>158</v>
       </c>
       <c r="D5" s="41" t="s">
         <v>157</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>168</v>
+        <v>459</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>58</v>
       </c>
-      <c r="G5" s="35" t="s">
-        <v>167</v>
-      </c>
-      <c r="H5" s="32"/>
+      <c r="G5" s="46" t="s">
+        <v>464</v>
+      </c>
+      <c r="H5" s="171" t="s">
+        <v>468</v>
+      </c>
       <c r="I5" s="47">
         <v>0</v>
       </c>
-      <c r="J5" s="32"/>
-      <c r="K5" s="32"/>
+      <c r="J5" s="169" t="s">
+        <v>430</v>
+      </c>
+      <c r="K5" s="170" t="s">
+        <v>432</v>
+      </c>
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
@@ -13516,19 +13738,19 @@
         <v>151</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>169</v>
+        <v>162</v>
       </c>
       <c r="D6" s="41" t="s">
         <v>157</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="47">
@@ -13538,28 +13760,60 @@
       <c r="K6" s="32"/>
     </row>
     <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="32"/>
-      <c r="B7" s="32"/>
-      <c r="C7" s="44"/>
-      <c r="D7" s="41"/>
-      <c r="E7" s="35"/>
-      <c r="F7" s="37"/>
-      <c r="G7" s="35"/>
+      <c r="A7" s="32" t="s">
+        <v>465</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C7" s="44" t="s">
+        <v>163</v>
+      </c>
+      <c r="D7" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="E7" s="35" t="s">
+        <v>165</v>
+      </c>
+      <c r="F7" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="G7" s="35" t="s">
+        <v>164</v>
+      </c>
       <c r="H7" s="32"/>
-      <c r="I7" s="47"/>
+      <c r="I7" s="47">
+        <v>0</v>
+      </c>
       <c r="J7" s="32"/>
       <c r="K7" s="32"/>
     </row>
     <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="32"/>
-      <c r="B8" s="32"/>
-      <c r="C8" s="32"/>
-      <c r="D8" s="41"/>
-      <c r="E8" s="35"/>
-      <c r="F8" s="40"/>
-      <c r="G8" s="35"/>
+      <c r="A8" s="32" t="s">
+        <v>466</v>
+      </c>
+      <c r="B8" s="32" t="s">
+        <v>151</v>
+      </c>
+      <c r="C8" s="44" t="s">
+        <v>166</v>
+      </c>
+      <c r="D8" s="41" t="s">
+        <v>157</v>
+      </c>
+      <c r="E8" s="35" t="s">
+        <v>168</v>
+      </c>
+      <c r="F8" s="37" t="s">
+        <v>58</v>
+      </c>
+      <c r="G8" s="35" t="s">
+        <v>167</v>
+      </c>
       <c r="H8" s="32"/>
-      <c r="I8" s="47"/>
+      <c r="I8" s="47">
+        <v>1</v>
+      </c>
       <c r="J8" s="32"/>
       <c r="K8" s="32"/>
     </row>
@@ -13903,25 +14157,25 @@
     </row>
     <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>173</v>
+        <v>169</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>193</v>
+        <v>189</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="47">
@@ -13932,25 +14186,25 @@
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
+        <v>170</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>174</v>
       </c>
-      <c r="B3" s="32" t="s">
-        <v>178</v>
-      </c>
       <c r="C3" s="44" t="s">
-        <v>183</v>
+        <v>179</v>
       </c>
       <c r="D3" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>185</v>
+        <v>181</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>181</v>
+        <v>177</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="47">
@@ -13961,25 +14215,25 @@
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
+        <v>171</v>
+      </c>
+      <c r="B4" s="32" t="s">
+        <v>174</v>
+      </c>
+      <c r="C4" s="44" t="s">
+        <v>188</v>
+      </c>
+      <c r="D4" s="41" t="s">
         <v>175</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>178</v>
-      </c>
-      <c r="C4" s="44" t="s">
-        <v>192</v>
-      </c>
-      <c r="D4" s="41" t="s">
-        <v>179</v>
-      </c>
       <c r="E4" s="35" t="s">
-        <v>187</v>
+        <v>183</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="47">
@@ -13990,25 +14244,25 @@
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>191</v>
+        <v>187</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>184</v>
+        <v>180</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>180</v>
+        <v>176</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="47">
@@ -14019,25 +14273,25 @@
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>177</v>
+        <v>173</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>178</v>
+        <v>174</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>190</v>
+        <v>186</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>188</v>
+        <v>184</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="47">
@@ -14410,25 +14664,25 @@
     </row>
     <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>195</v>
+        <v>191</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>201</v>
+        <v>197</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E2" s="35" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F2" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="47">
@@ -14439,25 +14693,25 @@
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
+        <v>192</v>
+      </c>
+      <c r="B3" s="32" t="s">
         <v>196</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="C3" s="44" t="s">
+        <v>212</v>
+      </c>
+      <c r="D3" s="41" t="s">
         <v>200</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>216</v>
-      </c>
-      <c r="D3" s="41" t="s">
-        <v>204</v>
-      </c>
       <c r="E3" s="35" t="s">
-        <v>205</v>
+        <v>201</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="47">
@@ -14468,25 +14722,25 @@
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
-        <v>197</v>
+        <v>193</v>
       </c>
       <c r="B4" s="32" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C4" s="44" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="47">
@@ -14497,25 +14751,25 @@
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>198</v>
+        <v>194</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>209</v>
+        <v>205</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>207</v>
+        <v>203</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="47">
@@ -14526,25 +14780,25 @@
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>199</v>
+        <v>195</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>210</v>
+        <v>206</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>206</v>
+        <v>202</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>211</v>
+        <v>207</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>213</v>
+        <v>209</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="47">
@@ -14555,25 +14809,25 @@
     </row>
     <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>200</v>
+        <v>196</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>219</v>
+        <v>215</v>
       </c>
       <c r="F7" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>220</v>
+        <v>216</v>
       </c>
       <c r="H7" s="32"/>
       <c r="I7" s="47">
@@ -14935,16 +15189,16 @@
     </row>
     <row r="2" spans="1:11" s="33" customFormat="1" ht="116.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
-        <v>221</v>
+        <v>217</v>
       </c>
       <c r="B2" s="32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C2" s="44" t="s">
-        <v>232</v>
+        <v>228</v>
       </c>
       <c r="D2" s="41" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="E2" s="35" t="s">
         <v>43</v>
@@ -14953,7 +15207,7 @@
         <v>44</v>
       </c>
       <c r="G2" s="35" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="H2" s="32"/>
       <c r="I2" s="47">
@@ -14964,25 +15218,25 @@
     </row>
     <row r="3" spans="1:11" s="33" customFormat="1" ht="117.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="32" t="s">
-        <v>222</v>
+        <v>218</v>
       </c>
       <c r="B3" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C3" s="44" t="s">
         <v>227</v>
       </c>
-      <c r="C3" s="44" t="s">
-        <v>231</v>
-      </c>
       <c r="D3" s="41" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E3" s="35" t="s">
-        <v>233</v>
+        <v>229</v>
       </c>
       <c r="F3" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G3" s="35" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H3" s="32"/>
       <c r="I3" s="47">
@@ -14993,25 +15247,25 @@
     </row>
     <row r="4" spans="1:11" s="33" customFormat="1" ht="133.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
+        <v>219</v>
+      </c>
+      <c r="B4" s="32" t="s">
         <v>223</v>
       </c>
-      <c r="B4" s="32" t="s">
-        <v>227</v>
-      </c>
       <c r="C4" s="44" t="s">
-        <v>238</v>
+        <v>234</v>
       </c>
       <c r="D4" s="41" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E4" s="35" t="s">
-        <v>234</v>
+        <v>230</v>
       </c>
       <c r="F4" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G4" s="35" t="s">
-        <v>230</v>
+        <v>226</v>
       </c>
       <c r="H4" s="32"/>
       <c r="I4" s="47">
@@ -15022,25 +15276,25 @@
     </row>
     <row r="5" spans="1:11" s="33" customFormat="1" ht="142.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="32" t="s">
-        <v>224</v>
+        <v>220</v>
       </c>
       <c r="B5" s="32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C5" s="44" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="D5" s="41" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E5" s="35" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="F5" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G5" s="35" t="s">
-        <v>235</v>
+        <v>231</v>
       </c>
       <c r="H5" s="32"/>
       <c r="I5" s="47">
@@ -15051,25 +15305,25 @@
     </row>
     <row r="6" spans="1:11" s="33" customFormat="1" ht="129" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="32" t="s">
-        <v>225</v>
+        <v>221</v>
       </c>
       <c r="B6" s="32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C6" s="44" t="s">
-        <v>237</v>
+        <v>233</v>
       </c>
       <c r="D6" s="41" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E6" s="35" t="s">
-        <v>246</v>
+        <v>242</v>
       </c>
       <c r="F6" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G6" s="35" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="H6" s="32"/>
       <c r="I6" s="47">
@@ -15080,25 +15334,25 @@
     </row>
     <row r="7" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="32" t="s">
-        <v>226</v>
+        <v>222</v>
       </c>
       <c r="B7" s="32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C7" s="44" t="s">
-        <v>242</v>
+        <v>238</v>
       </c>
       <c r="D7" s="41" t="s">
-        <v>204</v>
+        <v>200</v>
       </c>
       <c r="E7" s="35" t="s">
-        <v>241</v>
+        <v>237</v>
       </c>
       <c r="F7" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G7" s="35" t="s">
-        <v>240</v>
+        <v>236</v>
       </c>
       <c r="H7" s="32"/>
       <c r="I7" s="47">
@@ -15109,13 +15363,13 @@
     </row>
     <row r="8" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
-        <v>243</v>
+        <v>239</v>
       </c>
       <c r="B8" s="32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C8" s="32" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="D8" s="41" t="s">
         <v>109</v>
@@ -15138,25 +15392,25 @@
     </row>
     <row r="9" spans="1:11" s="33" customFormat="1" ht="127.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="32" t="s">
+        <v>240</v>
+      </c>
+      <c r="B9" s="32" t="s">
+        <v>223</v>
+      </c>
+      <c r="C9" s="44" t="s">
         <v>244</v>
       </c>
-      <c r="B9" s="32" t="s">
-        <v>227</v>
-      </c>
-      <c r="C9" s="44" t="s">
-        <v>248</v>
-      </c>
       <c r="D9" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E9" s="35" t="s">
-        <v>186</v>
+        <v>182</v>
       </c>
       <c r="F9" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G9" s="35" t="s">
-        <v>182</v>
+        <v>178</v>
       </c>
       <c r="H9" s="32"/>
       <c r="I9" s="47">
@@ -15167,25 +15421,25 @@
     </row>
     <row r="10" spans="1:11" s="33" customFormat="1" ht="103.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="32" t="s">
-        <v>245</v>
+        <v>241</v>
       </c>
       <c r="B10" s="32" t="s">
-        <v>227</v>
+        <v>223</v>
       </c>
       <c r="C10" s="44" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="D10" s="41" t="s">
-        <v>179</v>
+        <v>175</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>202</v>
+        <v>198</v>
       </c>
       <c r="F10" s="37" t="s">
         <v>58</v>
       </c>
       <c r="G10" s="35" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="H10" s="32"/>
       <c r="I10" s="47">

</xml_diff>